<commit_message>
Delete .csv, Update .xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,41 +488,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sweets</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Chocolate</t>
+          <t>Nectarines</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Chocolate</t>
+          <t>Healthy - Fruit - Nectarines</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F2" t="n">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G2" t="n">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="H2" t="n">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="I2" t="n">
-        <v>210</v>
+        <v>165</v>
       </c>
       <c r="J2" t="n">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -538,111 +538,111 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Cake</t>
+          <t>Ice Cream</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Cake</t>
+          <t>Unhealthy - Sweets - Ice Cream</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F3" t="n">
-        <v>55</v>
+        <v>173</v>
       </c>
       <c r="G3" t="n">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="H3" t="n">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="I3" t="n">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="J3" t="n">
-        <v>92</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dairy</t>
+          <t>Fats</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yogurt</t>
+          <t>Olive Oil</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Healthy - Dairy - Yogurt</t>
+          <t>Unhealthy - Fats - Olive Oil</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="G4" t="n">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="H4" t="n">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="I4" t="n">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="J4" t="n">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Fats</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Nectarines</t>
+          <t>Avacado Oil</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Nectarines</t>
+          <t>Unhealthy - Fats - Avacado Oil</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="F5" t="n">
-        <v>123</v>
+        <v>25</v>
       </c>
       <c r="G5" t="n">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="H5" t="n">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="I5" t="n">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="J5" t="n">
-        <v>62</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
@@ -658,151 +658,151 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pie</t>
+          <t>Pudding</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Pie</t>
+          <t>Unhealthy - Sweets - Pudding</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F6" t="n">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="G6" t="n">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="H6" t="n">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="I6" t="n">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="J6" t="n">
-        <v>120</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fats</t>
+          <t>Dairy</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Grape Seed Oil</t>
+          <t>Cheese</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Unhealthy - Fats - Grape Seed Oil</t>
+          <t>Healthy - Dairy - Cheese</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="F7" t="n">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="G7" t="n">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="H7" t="n">
         <v>22</v>
       </c>
       <c r="I7" t="n">
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="J7" t="n">
-        <v>23</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fats</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Avacado Oil</t>
+          <t>Artichokes</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Unhealthy - Fats - Avacado Oil</t>
+          <t>Healthy - Vegetable - Artichokes</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="F8" t="n">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="G8" t="n">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="H8" t="n">
         <v>24</v>
       </c>
       <c r="I8" t="n">
-        <v>72</v>
+        <v>158</v>
       </c>
       <c r="J8" t="n">
-        <v>106</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Fats</t>
+          <t>Dairy</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Olive Oil</t>
+          <t>Milk</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Unhealthy - Fats - Olive Oil</t>
+          <t>Healthy - Dairy - Milk</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="F9" t="n">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="G9" t="n">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="H9" t="n">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="I9" t="n">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="J9" t="n">
-        <v>111</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -813,36 +813,36 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Beef</t>
+          <t>Guava</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Beef</t>
+          <t>Healthy - Fruit - Guava</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F10" t="n">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="G10" t="n">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="H10" t="n">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="I10" t="n">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="J10" t="n">
-        <v>73</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11">
@@ -867,102 +867,102 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="F11" t="n">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G11" t="n">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="H11" t="n">
-        <v>53</v>
+        <v>162</v>
       </c>
       <c r="I11" t="n">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="J11" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Sweets</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Zucchini</t>
+          <t>Cookies</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Zucchini</t>
+          <t>Unhealthy - Sweets - Cookies</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>139</v>
+        <v>62</v>
       </c>
       <c r="F12" t="n">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G12" t="n">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="H12" t="n">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="I12" t="n">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="J12" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Fats</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Venison</t>
+          <t>Butter</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Venison</t>
+          <t>Unhealthy - Fats - Butter</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="G13" t="n">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="H13" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="I13" t="n">
-        <v>229</v>
+        <v>67</v>
       </c>
       <c r="J13" t="n">
-        <v>26</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14">
@@ -973,36 +973,36 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Grain</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Quinoa</t>
+          <t>Peach</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Healthy - Grain - Quinoa</t>
+          <t>Healthy - Fruit - Peach</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F14" t="n">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="G14" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H14" t="n">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="I14" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="J14" t="n">
-        <v>131</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -1013,116 +1013,116 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Dairy</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Broccoli</t>
+          <t>Yogurt</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Broccoli</t>
+          <t>Healthy - Dairy - Yogurt</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="F15" t="n">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="G15" t="n">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="H15" t="n">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="I15" t="n">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="J15" t="n">
-        <v>117</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Fats</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Cucumber</t>
+          <t>Grape Seed Oil</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Cucumber</t>
+          <t>Unhealthy - Fats - Grape Seed Oil</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="F16" t="n">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="G16" t="n">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="H16" t="n">
         <v>125</v>
       </c>
       <c r="I16" t="n">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="J16" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sweets</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cookies</t>
+          <t>Peas</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Cookies</t>
+          <t>Healthy - Vegetable - Peas</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="F17" t="n">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="G17" t="n">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="H17" t="n">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="I17" t="n">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="J17" t="n">
-        <v>3</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
@@ -1133,76 +1133,76 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Grain</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Rye</t>
+          <t>Plum</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Healthy - Grain - Rye</t>
+          <t>Healthy - Fruit - Plum</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>221</v>
+        <v>68</v>
       </c>
       <c r="F18" t="n">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="G18" t="n">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="H18" t="n">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="I18" t="n">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="J18" t="n">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Fats</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Butter</t>
+          <t>Lamb</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Unhealthy - Fats - Butter</t>
+          <t>Healthy - Meat - Lamb</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="F19" t="n">
-        <v>154</v>
+        <v>95</v>
       </c>
       <c r="G19" t="n">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="H19" t="n">
-        <v>47</v>
+        <v>171</v>
       </c>
       <c r="I19" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J19" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -1213,76 +1213,76 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Grain</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Duck</t>
+          <t>Oats</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Duck</t>
+          <t>Healthy - Grain - Oats</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="F20" t="n">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="G20" t="n">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="H20" t="n">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="I20" t="n">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="J20" t="n">
-        <v>117</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sweets</t>
+          <t>Grain</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Donuts</t>
+          <t>Barley</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Donuts</t>
+          <t>Healthy - Grain - Barley</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="F21" t="n">
-        <v>147</v>
+        <v>23</v>
       </c>
       <c r="G21" t="n">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="I21" t="n">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="J21" t="n">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22">
@@ -1298,71 +1298,71 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Pudding</t>
+          <t>Candy</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Pudding</t>
+          <t>Unhealthy - Sweets - Candy</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="F22" t="n">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G22" t="n">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="H22" t="n">
-        <v>105</v>
+        <v>188</v>
       </c>
       <c r="I22" t="n">
-        <v>189</v>
+        <v>60</v>
       </c>
       <c r="J22" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Unhealthy</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sweets</t>
+          <t>Grain</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ice Cream</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Ice Cream</t>
+          <t>Healthy - Grain - Rice</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>150</v>
+        <v>31</v>
       </c>
       <c r="F23" t="n">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="G23" t="n">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="H23" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I23" t="n">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="J23" t="n">
-        <v>119</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24">
@@ -1373,76 +1373,76 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Grapes</t>
+          <t>Asparagus</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Grapes</t>
+          <t>Healthy - Vegetable - Asparagus</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="F24" t="n">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="G24" t="n">
-        <v>192</v>
+        <v>51</v>
       </c>
       <c r="H24" t="n">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="I24" t="n">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="J24" t="n">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Sweets</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tomato</t>
+          <t>Chocolate</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Tomato</t>
+          <t>Unhealthy - Sweets - Chocolate</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="F25" t="n">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="G25" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H25" t="n">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="I25" t="n">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="J25" t="n">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26">
@@ -1458,71 +1458,71 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Candy</t>
+          <t>Pie</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Unhealthy - Sweets - Candy</t>
+          <t>Unhealthy - Sweets - Pie</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="F26" t="n">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="G26" t="n">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H26" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="I26" t="n">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="J26" t="n">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Sweets</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Peas</t>
+          <t>Donuts</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Peas</t>
+          <t>Unhealthy - Sweets - Donuts</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="F27" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G27" t="n">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="H27" t="n">
-        <v>131</v>
+        <v>48</v>
       </c>
       <c r="I27" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J27" t="n">
-        <v>125</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28">
@@ -1533,36 +1533,36 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Dairy</t>
+          <t>Grain</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cheese</t>
+          <t>Rye</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Healthy - Dairy - Cheese</t>
+          <t>Healthy - Grain - Rye</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>194</v>
+        <v>59</v>
       </c>
       <c r="F28" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="G28" t="n">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="H28" t="n">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="I28" t="n">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="J28" t="n">
-        <v>201</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29">
@@ -1573,36 +1573,36 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Orange</t>
+          <t>Healthy - Meat - Turkey</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="F29" t="n">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="G29" t="n">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="H29" t="n">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="I29" t="n">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="J29" t="n">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30">
@@ -1613,36 +1613,36 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Plant-based Protein</t>
+          <t>Grain</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Beans</t>
+          <t>Corn</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Healthy - Plant-based Protein - Beans</t>
+          <t>Healthy - Grain - Corn</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="F30" t="n">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="G30" t="n">
-        <v>181</v>
+        <v>109</v>
       </c>
       <c r="H30" t="n">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="I30" t="n">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="J30" t="n">
-        <v>2</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31">
@@ -1653,36 +1653,36 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Plant-based Protein</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Carrots</t>
+          <t>Seitan</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Carrots</t>
+          <t>Healthy - Plant-based Protein - Seitan</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="F31" t="n">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G31" t="n">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="H31" t="n">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="I31" t="n">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="J31" t="n">
-        <v>136</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32">
@@ -1693,36 +1693,36 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Dairy</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Rabbit</t>
+          <t>Cream</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Rabbit</t>
+          <t>Healthy - Dairy - Cream</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="F32" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="G32" t="n">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H32" t="n">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I32" t="n">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="J32" t="n">
-        <v>45</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33">
@@ -1733,36 +1733,36 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Guava</t>
+          <t>Chicken</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Guava</t>
+          <t>Healthy - Meat - Chicken</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="F33" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="G33" t="n">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="H33" t="n">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="I33" t="n">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="J33" t="n">
-        <v>103</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34">
@@ -1773,36 +1773,36 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Beets</t>
+          <t>Eggs</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Beets</t>
+          <t>Healthy - Meat - Eggs</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F34" t="n">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G34" t="n">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H34" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I34" t="n">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="J34" t="n">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35">
@@ -1813,36 +1813,36 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Melon</t>
+          <t>Quail</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Melon</t>
+          <t>Healthy - Meat - Quail</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F35" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G35" t="n">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="H35" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I35" t="n">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="J35" t="n">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36">
@@ -1853,36 +1853,36 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cabbage</t>
+          <t>Pear</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Cabbage</t>
+          <t>Healthy - Fruit - Pear</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="F36" t="n">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="G36" t="n">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="H36" t="n">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="I36" t="n">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="J36" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37">
@@ -1893,36 +1893,36 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Grain</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Corn</t>
+          <t>Grapes</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Healthy - Grain - Corn</t>
+          <t>Healthy - Fruit - Grapes</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="F37" t="n">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="G37" t="n">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="H37" t="n">
-        <v>143</v>
+        <v>42</v>
       </c>
       <c r="I37" t="n">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="J37" t="n">
-        <v>81</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38">
@@ -1947,22 +1947,22 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="F38" t="n">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="G38" t="n">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="H38" t="n">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="I38" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J38" t="n">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39">
@@ -1973,36 +1973,36 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Eggs</t>
+          <t>Squash</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Eggs</t>
+          <t>Healthy - Vegetable - Squash</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="F39" t="n">
+        <v>8</v>
+      </c>
+      <c r="G39" t="n">
+        <v>54</v>
+      </c>
+      <c r="H39" t="n">
+        <v>64</v>
+      </c>
+      <c r="I39" t="n">
+        <v>177</v>
+      </c>
+      <c r="J39" t="n">
         <v>82</v>
-      </c>
-      <c r="G39" t="n">
-        <v>43</v>
-      </c>
-      <c r="H39" t="n">
-        <v>88</v>
-      </c>
-      <c r="I39" t="n">
-        <v>88</v>
-      </c>
-      <c r="J39" t="n">
-        <v>134</v>
       </c>
     </row>
     <row r="40">
@@ -2018,31 +2018,31 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Strawberries</t>
+          <t>Melon</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Strawberries</t>
+          <t>Healthy - Fruit - Melon</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="F40" t="n">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="G40" t="n">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="H40" t="n">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="I40" t="n">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="J40" t="n">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41">
@@ -2053,36 +2053,36 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Goose</t>
+          <t>Papaya</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Goose</t>
+          <t>Healthy - Fruit - Papaya</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>150</v>
+        <v>62</v>
       </c>
       <c r="F41" t="n">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="G41" t="n">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="H41" t="n">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="I41" t="n">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="J41" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
@@ -2093,36 +2093,36 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Mango</t>
+          <t>Bell Peppers</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Mango</t>
+          <t>Healthy - Vegetable - Bell Peppers</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="G42" t="n">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="H42" t="n">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="I42" t="n">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J42" t="n">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43">
@@ -2133,36 +2133,36 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Grain</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Potato</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Healthy - Grain - Rice</t>
+          <t>Healthy - Vegetable - Potato</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="F43" t="n">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="G43" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="I43" t="n">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="J43" t="n">
-        <v>59</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44">
@@ -2178,31 +2178,31 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Apricots</t>
+          <t>Banana</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Apricots</t>
+          <t>Healthy - Fruit - Banana</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="F44" t="n">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="G44" t="n">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H44" t="n">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="I44" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J44" t="n">
-        <v>42</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45">
@@ -2213,36 +2213,36 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Grain</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Asparagus</t>
+          <t>Quinoa</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Asparagus</t>
+          <t>Healthy - Grain - Quinoa</t>
         </is>
       </c>
       <c r="E45" t="n">
         <v>102</v>
       </c>
       <c r="F45" t="n">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="G45" t="n">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="H45" t="n">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="I45" t="n">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="J45" t="n">
-        <v>53</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
@@ -2253,36 +2253,36 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Plant-based Protein</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Nuts and Seeds</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Healthy - Plant-based Protein - Nuts and Seeds</t>
+          <t>Healthy - Fruit - Orange</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>140</v>
+        <v>72</v>
       </c>
       <c r="F46" t="n">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="G46" t="n">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="H46" t="n">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="I46" t="n">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="J46" t="n">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47">
@@ -2293,36 +2293,36 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Pork</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Apple</t>
+          <t>Healthy - Meat - Pork</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="F47" t="n">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="G47" t="n">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="H47" t="n">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="I47" t="n">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="J47" t="n">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48">
@@ -2333,36 +2333,36 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Plant-based Protein</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Banana</t>
+          <t>Beans</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Banana</t>
+          <t>Healthy - Plant-based Protein - Beans</t>
         </is>
       </c>
       <c r="E48" t="n">
+        <v>85</v>
+      </c>
+      <c r="F48" t="n">
         <v>122</v>
       </c>
-      <c r="F48" t="n">
-        <v>97</v>
-      </c>
       <c r="G48" t="n">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="H48" t="n">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="I48" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="J48" t="n">
-        <v>130</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49">
@@ -2373,76 +2373,76 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Egg Plant</t>
+          <t>Beef</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Egg Plant</t>
+          <t>Healthy - Meat - Beef</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F49" t="n">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="G49" t="n">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H49" t="n">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I49" t="n">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="J49" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Unhealthy</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Sweets</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Cake</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Fish</t>
+          <t>Unhealthy - Sweets - Cake</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="F50" t="n">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="G50" t="n">
-        <v>192</v>
+        <v>65</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I50" t="n">
-        <v>199</v>
+        <v>53</v>
       </c>
       <c r="J50" t="n">
-        <v>16</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51">
@@ -2453,36 +2453,36 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Grain</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Barley</t>
+          <t>Mango</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Healthy - Grain - Barley</t>
+          <t>Healthy - Fruit - Mango</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="F51" t="n">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="G51" t="n">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="H51" t="n">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I51" t="n">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="J51" t="n">
-        <v>144</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52">
@@ -2493,36 +2493,36 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Plant-based Protein</t>
+          <t>Grain</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Seitan</t>
+          <t>Wheat</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Healthy - Plant-based Protein - Seitan</t>
+          <t>Healthy - Grain - Wheat</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="F52" t="n">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="G52" t="n">
-        <v>194</v>
+        <v>36</v>
       </c>
       <c r="H52" t="n">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="I52" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="J52" t="n">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53">
@@ -2533,36 +2533,36 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Grain</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Oats</t>
+          <t>Goose</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Healthy - Grain - Oats</t>
+          <t>Healthy - Meat - Goose</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>37</v>
+        <v>172</v>
       </c>
       <c r="F53" t="n">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="G53" t="n">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="H53" t="n">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="I53" t="n">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="J53" t="n">
-        <v>130</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54">
@@ -2573,36 +2573,36 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Plant-based Protein</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Tofu</t>
+          <t>Spinach</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Healthy - Plant-based Protein - Tofu</t>
+          <t>Healthy - Vegetable - Spinach</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="F54" t="n">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="G54" t="n">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="H54" t="n">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="I54" t="n">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="J54" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55">
@@ -2613,36 +2613,36 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Grain</t>
+          <t>Plant-based Protein</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Wheat</t>
+          <t>Chickpeas</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Healthy - Grain - Wheat</t>
+          <t>Healthy - Plant-based Protein - Chickpeas</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F55" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="G55" t="n">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="H55" t="n">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="I55" t="n">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="J55" t="n">
-        <v>110</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56">
@@ -2653,36 +2653,36 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Dairy</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Cream</t>
+          <t>Carrots</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Healthy - Dairy - Cream</t>
+          <t>Healthy - Vegetable - Carrots</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="G56" t="n">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="H56" t="n">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="I56" t="n">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="J56" t="n">
-        <v>92</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57">
@@ -2698,31 +2698,31 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Squash</t>
+          <t>Lettuce</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Squash</t>
+          <t>Healthy - Vegetable - Lettuce</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>123</v>
+        <v>29</v>
       </c>
       <c r="F57" t="n">
-        <v>156</v>
+        <v>8</v>
       </c>
       <c r="G57" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="H57" t="n">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="I57" t="n">
-        <v>153</v>
+        <v>75</v>
       </c>
       <c r="J57" t="n">
-        <v>50</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58">
@@ -2733,36 +2733,36 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Dairy</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Milk</t>
+          <t>Duck</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Healthy - Dairy - Milk</t>
+          <t>Healthy - Meat - Duck</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>201</v>
+        <v>42</v>
       </c>
       <c r="F58" t="n">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="G58" t="n">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="H58" t="n">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="I58" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J58" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59">
@@ -2773,36 +2773,36 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Chicken</t>
+          <t>Apricots</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Chicken</t>
+          <t>Healthy - Fruit - Apricots</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>67</v>
+        <v>161</v>
       </c>
       <c r="F59" t="n">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="G59" t="n">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="H59" t="n">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="I59" t="n">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="J59" t="n">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60">
@@ -2813,36 +2813,36 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Pear</t>
+          <t>Egg Plant</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Pear</t>
+          <t>Healthy - Vegetable - Egg Plant</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="F60" t="n">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="G60" t="n">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H60" t="n">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="I60" t="n">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="J60" t="n">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61">
@@ -2853,36 +2853,36 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Cauliflower</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Cauliflower</t>
+          <t>Healthy - Fruit - Apple</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="F61" t="n">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="G61" t="n">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="H61" t="n">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="I61" t="n">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="J61" t="n">
-        <v>7</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62">
@@ -2898,31 +2898,31 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Spinach</t>
+          <t>Broccoli</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Spinach</t>
+          <t>Healthy - Vegetable - Broccoli</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="F62" t="n">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="G62" t="n">
-        <v>155</v>
+        <v>88</v>
       </c>
       <c r="H62" t="n">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="I62" t="n">
-        <v>156</v>
+        <v>76</v>
       </c>
       <c r="J62" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63">
@@ -2933,36 +2933,36 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Meat</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Potato</t>
+          <t>Fish</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Potato</t>
+          <t>Healthy - Meat - Fish</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="G63" t="n">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="H63" t="n">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="I63" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="J63" t="n">
-        <v>125</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64">
@@ -2978,31 +2978,31 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Pork</t>
+          <t>Venison</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Pork</t>
+          <t>Healthy - Meat - Venison</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="F64" t="n">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="G64" t="n">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="H64" t="n">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="I64" t="n">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="J64" t="n">
-        <v>82</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65">
@@ -3013,36 +3013,36 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Plant-based Protein</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Lamb</t>
+          <t>Nuts and Seeds</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Lamb</t>
+          <t>Healthy - Plant-based Protein - Nuts and Seeds</t>
         </is>
       </c>
       <c r="E65" t="n">
+        <v>48</v>
+      </c>
+      <c r="F65" t="n">
+        <v>158</v>
+      </c>
+      <c r="G65" t="n">
         <v>67</v>
       </c>
-      <c r="F65" t="n">
-        <v>13</v>
-      </c>
-      <c r="G65" t="n">
-        <v>213</v>
-      </c>
       <c r="H65" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="I65" t="n">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="J65" t="n">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66">
@@ -3053,36 +3053,36 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Cherry</t>
+          <t>Cabbage</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Cherry</t>
+          <t>Healthy - Vegetable - Cabbage</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="F66" t="n">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="G66" t="n">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="H66" t="n">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="I66" t="n">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="J66" t="n">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67">
@@ -3093,36 +3093,36 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Quail</t>
+          <t>Pineapples</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Quail</t>
+          <t>Healthy - Fruit - Pineapples</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="F67" t="n">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="G67" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H67" t="n">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="I67" t="n">
-        <v>2</v>
+        <v>146</v>
       </c>
       <c r="J67" t="n">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68">
@@ -3133,36 +3133,36 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Plant-based Protein</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Lettuce</t>
+          <t>Tofu</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Lettuce</t>
+          <t>Healthy - Plant-based Protein - Tofu</t>
         </is>
       </c>
       <c r="E68" t="n">
+        <v>49</v>
+      </c>
+      <c r="F68" t="n">
+        <v>16</v>
+      </c>
+      <c r="G68" t="n">
+        <v>132</v>
+      </c>
+      <c r="H68" t="n">
+        <v>126</v>
+      </c>
+      <c r="I68" t="n">
         <v>111</v>
       </c>
-      <c r="F68" t="n">
-        <v>38</v>
-      </c>
-      <c r="G68" t="n">
-        <v>111</v>
-      </c>
-      <c r="H68" t="n">
-        <v>77</v>
-      </c>
-      <c r="I68" t="n">
-        <v>43</v>
-      </c>
       <c r="J68" t="n">
-        <v>117</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69">
@@ -3173,36 +3173,36 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Papaya</t>
+          <t>Tomato</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Papaya</t>
+          <t>Healthy - Vegetable - Tomato</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="F69" t="n">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="G69" t="n">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="H69" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I69" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="J69" t="n">
-        <v>95</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70">
@@ -3213,36 +3213,36 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Meat</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Onion</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Healthy - Meat - Turkey</t>
+          <t>Healthy - Vegetable - Onion</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="F70" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="G70" t="n">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="H70" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I70" t="n">
-        <v>177</v>
+        <v>103</v>
       </c>
       <c r="J70" t="n">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71">
@@ -3253,36 +3253,36 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Plant-based Protein</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Chickpeas</t>
+          <t>Beets</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Healthy - Plant-based Protein - Chickpeas</t>
+          <t>Healthy - Vegetable - Beets</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>122</v>
+        <v>32</v>
       </c>
       <c r="F71" t="n">
-        <v>191</v>
+        <v>16</v>
       </c>
       <c r="G71" t="n">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="H71" t="n">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="I71" t="n">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72">
@@ -3298,31 +3298,31 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Pineapples</t>
+          <t>Cherry</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Pineapples</t>
+          <t>Healthy - Fruit - Cherry</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="F72" t="n">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="G72" t="n">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H72" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I72" t="n">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="J72" t="n">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73">
@@ -3333,36 +3333,36 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Vegetable</t>
+          <t>Fruit</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Onion</t>
+          <t>Strawberries</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Onion</t>
+          <t>Healthy - Fruit - Strawberries</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="F73" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="G73" t="n">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="H73" t="n">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="I73" t="n">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="J73" t="n">
-        <v>88</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74">
@@ -3373,36 +3373,36 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Vegetable</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Peach</t>
+          <t>Corn</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Healthy - Fruit - Peach</t>
+          <t>Healthy - Vegetable - Corn</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>226</v>
+        <v>157</v>
       </c>
       <c r="F74" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="H74" t="n">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="I74" t="n">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="J74" t="n">
-        <v>128</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75">
@@ -3418,31 +3418,31 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Artichokes</t>
+          <t>Mushrooms</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Artichokes</t>
+          <t>Healthy - Vegetable - Mushrooms</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="F75" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="G75" t="n">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="H75" t="n">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="I75" t="n">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="J75" t="n">
-        <v>143</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76">
@@ -3458,31 +3458,151 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Mushrooms</t>
+          <t>Cucumber</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Healthy - Vegetable - Mushrooms</t>
+          <t>Healthy - Vegetable - Cucumber</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G76" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H76" t="n">
-        <v>125</v>
+        <v>32</v>
       </c>
       <c r="I76" t="n">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="J76" t="n">
-        <v>152</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Healthy</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Vegetable</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Zucchini</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Healthy - Vegetable - Zucchini</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>159</v>
+      </c>
+      <c r="F77" t="n">
+        <v>110</v>
+      </c>
+      <c r="G77" t="n">
+        <v>2</v>
+      </c>
+      <c r="H77" t="n">
+        <v>32</v>
+      </c>
+      <c r="I77" t="n">
+        <v>40</v>
+      </c>
+      <c r="J77" t="n">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Healthy</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Vegetable</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Cauliflower</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Healthy - Vegetable - Cauliflower</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>76</v>
+      </c>
+      <c r="F78" t="n">
+        <v>104</v>
+      </c>
+      <c r="G78" t="n">
+        <v>97</v>
+      </c>
+      <c r="H78" t="n">
+        <v>122</v>
+      </c>
+      <c r="I78" t="n">
+        <v>58</v>
+      </c>
+      <c r="J78" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Healthy</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Meat</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Rabbit</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Healthy - Meat - Rabbit</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>20</v>
+      </c>
+      <c r="F79" t="n">
+        <v>96</v>
+      </c>
+      <c r="G79" t="n">
+        <v>57</v>
+      </c>
+      <c r="H79" t="n">
+        <v>120</v>
+      </c>
+      <c r="I79" t="n">
+        <v>110</v>
+      </c>
+      <c r="J79" t="n">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>